<commit_message>
piccola correzione pk fk ml
</commit_message>
<xml_diff>
--- a/Serie_A/modello_logico/ml_serie_a_v2.xlsx
+++ b/Serie_A/modello_logico/ml_serie_a_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grego\Desktop\DATABASE-FSD1\Serie_A\modello_logico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A21837-8097-4D9C-9318-E3A18CCF9C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9834269-B608-4706-B43C-06CA9E0687F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{099B281A-DC79-42D9-AAD9-754F7DEF1577}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
   <si>
     <t>stagione</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>(FK)</t>
+  </si>
+  <si>
+    <t>(PK) (FK)</t>
   </si>
 </sst>
 </file>
@@ -406,15 +409,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -422,6 +416,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -738,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53854CA-F955-438D-854B-43CA509EE07B}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -763,26 +766,26 @@
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="21"/>
+      <c r="C2" s="27"/>
       <c r="D2" s="15"/>
       <c r="E2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="23"/>
-      <c r="H2" s="24" t="s">
+      <c r="G2" s="26"/>
+      <c r="H2" s="21" t="s">
         <v>26</v>
       </c>
       <c r="I2" s="17"/>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="21"/>
+      <c r="K2" s="27"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
@@ -790,7 +793,7 @@
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="22">
         <v>1</v>
       </c>
       <c r="E3" s="4"/>
@@ -798,7 +801,7 @@
       <c r="G3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="26"/>
+      <c r="H3" s="23"/>
       <c r="I3" s="7"/>
       <c r="J3" s="1" t="s">
         <v>8</v>
@@ -822,10 +825,10 @@
       <c r="G4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="27"/>
+      <c r="H4" s="24"/>
       <c r="I4" s="7"/>
       <c r="J4" s="1" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>29</v>
@@ -845,7 +848,7 @@
       <c r="G5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="27"/>
+      <c r="H5" s="24"/>
       <c r="I5" s="4"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
@@ -866,7 +869,7 @@
       <c r="G6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="27"/>
+      <c r="H6" s="24"/>
       <c r="I6" s="4"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1" t="s">
@@ -887,7 +890,7 @@
       <c r="G7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="27"/>
+      <c r="H7" s="24"/>
       <c r="I7" s="4"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1" t="s">
@@ -908,7 +911,7 @@
       <c r="G8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H8" s="27"/>
+      <c r="H8" s="24"/>
       <c r="I8" s="4"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1" t="s">
@@ -923,7 +926,7 @@
       <c r="G9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="27"/>
+      <c r="H9" s="24"/>
       <c r="I9" s="4"/>
       <c r="J9" s="1"/>
       <c r="K9" s="10" t="s">
@@ -938,7 +941,7 @@
       <c r="G10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="27"/>
+      <c r="H10" s="24"/>
       <c r="I10" s="4"/>
       <c r="J10" s="19" t="s">
         <v>26</v>
@@ -952,7 +955,7 @@
       <c r="G11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="27"/>
+      <c r="H11" s="24"/>
       <c r="I11" s="4"/>
       <c r="J11" s="3"/>
       <c r="K11" s="18">
@@ -967,12 +970,12 @@
       <c r="G12" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="27"/>
+      <c r="H12" s="24"/>
       <c r="I12" s="4"/>
-      <c r="J12" s="22" t="s">
+      <c r="J12" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="K12" s="23"/>
+      <c r="K12" s="26"/>
     </row>
     <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
@@ -982,7 +985,7 @@
       <c r="G13" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="H13" s="27"/>
+      <c r="H13" s="24"/>
       <c r="I13" s="4">
         <v>1</v>
       </c>
@@ -1003,7 +1006,7 @@
         <v>20</v>
       </c>
       <c r="H14" s="4"/>
-      <c r="I14" s="28"/>
+      <c r="I14" s="25"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1" t="s">
         <v>24</v>
@@ -1046,12 +1049,12 @@
       <c r="G17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H17" s="24"/>
+      <c r="H17" s="21"/>
       <c r="I17" s="4"/>
-      <c r="J17" s="22" t="s">
+      <c r="J17" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="K17" s="23"/>
+      <c r="K17" s="26"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
@@ -1133,10 +1136,10 @@
         <v>27</v>
       </c>
       <c r="E23" s="6"/>
-      <c r="F23" s="22" t="s">
+      <c r="F23" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="23"/>
+      <c r="G23" s="26"/>
       <c r="H23" s="4"/>
       <c r="I23" s="5"/>
     </row>
@@ -1144,9 +1147,7 @@
       <c r="A24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
         <v>0</v>
       </c>
@@ -1271,12 +1272,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="B2:C2"/>
     <mergeCell ref="J2:K2"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F23:G23"/>
     <mergeCell ref="J17:K17"/>
     <mergeCell ref="J12:K12"/>
-    <mergeCell ref="B2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Insert 10 Record Partita + Statistiche
</commit_message>
<xml_diff>
--- a/Serie_A/modello_logico/ml_serie_a_v2.xlsx
+++ b/Serie_A/modello_logico/ml_serie_a_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grego\Desktop\DATABASE-FSD1\Serie_A\modello_logico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9834269-B608-4706-B43C-06CA9E0687F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81340B8A-C0F7-4CE9-847E-9549F971BE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{099B281A-DC79-42D9-AAD9-754F7DEF1577}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
   <si>
     <t>stagione</t>
   </si>
@@ -170,9 +170,6 @@
   </si>
   <si>
     <t>(FK)</t>
-  </si>
-  <si>
-    <t>(PK) (FK)</t>
   </si>
 </sst>
 </file>
@@ -416,10 +413,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -741,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B53854CA-F955-438D-854B-43CA509EE07B}">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -766,10 +763,10 @@
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="27"/>
+      <c r="C2" s="26"/>
       <c r="D2" s="15"/>
       <c r="E2" s="2" t="s">
         <v>26</v>
@@ -777,15 +774,15 @@
       <c r="F2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="26"/>
+      <c r="G2" s="27"/>
       <c r="H2" s="21" t="s">
         <v>26</v>
       </c>
       <c r="I2" s="17"/>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="27"/>
+      <c r="K2" s="26"/>
     </row>
     <row r="3" spans="1:11" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
@@ -828,7 +825,7 @@
       <c r="H4" s="24"/>
       <c r="I4" s="7"/>
       <c r="J4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>29</v>
@@ -975,7 +972,7 @@
       <c r="J12" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="K12" s="26"/>
+      <c r="K12" s="27"/>
     </row>
     <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
@@ -1054,7 +1051,7 @@
       <c r="J17" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="K17" s="26"/>
+      <c r="K17" s="27"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
@@ -1139,7 +1136,7 @@
       <c r="F23" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="26"/>
+      <c r="G23" s="27"/>
       <c r="H23" s="4"/>
       <c r="I23" s="5"/>
     </row>
@@ -1159,7 +1156,7 @@
       <c r="D25" s="4"/>
       <c r="E25" s="4"/>
       <c r="F25" s="1" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>28</v>
@@ -1174,7 +1171,7 @@
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="1" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>29</v>
@@ -1188,7 +1185,7 @@
       <c r="A27" s="4"/>
       <c r="D27" s="4"/>
       <c r="F27" s="1" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>9</v>

</xml_diff>